<commit_message>
Adding NCAA Brackets to commit
</commit_message>
<xml_diff>
--- a/NCAA Brackets.xlsx
+++ b/NCAA Brackets.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\MSSA\Side Projects\BracketBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E88DB0A-ED21-4A3D-9DA6-E9EFEFD18CCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D35F6D5-35F5-4E37-8B4E-15C639CAEBD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="1" r:id="rId1"/>
     <sheet name="Images" sheetId="2" r:id="rId2"/>
     <sheet name="Seeds" sheetId="3" r:id="rId3"/>
     <sheet name="Input" sheetId="6" r:id="rId4"/>
+    <sheet name="C# Input Test" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="3" hidden="1">Input!$A$1:$O$66</definedName>
@@ -778,6 +779,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -803,10 +808,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2591,7 +2592,7 @@
   </sheetPr>
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -3840,14 +3841,14 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="34" t="str">
+      <c r="I30" s="36" t="str">
         <f ca="1">I18</f>
         <v/>
       </c>
       <c r="J30" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="K30" s="34" t="str">
+      <c r="K30" s="36" t="str">
         <f ca="1">K18</f>
         <v/>
       </c>
@@ -3888,11 +3889,11 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="35"/>
+      <c r="I31" s="37"/>
       <c r="J31" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="K31" s="35"/>
+      <c r="K31" s="37"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -3980,7 +3981,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="6"/>
-      <c r="J33" s="34" t="str">
+      <c r="J33" s="36" t="str">
         <f ca="1">_xlfn.IFS(I32&gt;I37,I30,I32&lt;I37,I38,I32="","")&amp;IF(J32="","",(" ("&amp;J32&amp;")"))</f>
         <v/>
       </c>
@@ -4017,7 +4018,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="35"/>
+      <c r="J34" s="37"/>
       <c r="K34" s="7"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -4047,7 +4048,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="6"/>
-      <c r="J35" s="34" t="str">
+      <c r="J35" s="36" t="str">
         <f ca="1">_xlfn.IFS(K32&gt;K37,K30,K32&lt;K37,K38,K32="","")&amp;IF(J37="","",(" ("&amp;J37&amp;")"))</f>
         <v/>
       </c>
@@ -4086,7 +4087,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="6"/>
-      <c r="J36" s="35"/>
+      <c r="J36" s="37"/>
       <c r="K36" s="7"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -4174,12 +4175,12 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="34" t="str">
+      <c r="I38" s="36" t="str">
         <f ca="1">I51</f>
         <v/>
       </c>
       <c r="J38" s="1"/>
-      <c r="K38" s="34" t="str">
+      <c r="K38" s="36" t="str">
         <f ca="1">K51</f>
         <v/>
       </c>
@@ -4220,9 +4221,9 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="35"/>
+      <c r="I39" s="37"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="35"/>
+      <c r="K39" s="37"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1" t="str" cm="1">
@@ -4383,7 +4384,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="37" t="str" cm="1">
+      <c r="L43" s="28" t="str" cm="1">
         <f t="array" aca="1" ref="L43" ca="1">IF($H$1,INDIRECT("Input!J"&amp;Seeds!F99),"")</f>
         <v/>
       </c>
@@ -4460,11 +4461,11 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="27" t="s">
+      <c r="I45" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J45" s="28"/>
-      <c r="K45" s="29"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="31"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -4502,12 +4503,12 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="30" t="str">
+      <c r="I46" s="32" t="str">
         <f ca="1">_xlfn.IFS(J32&gt;J37,LEFT(J33,FIND("(",J33)-1),J32&lt;J37,LEFT(J35,FIND("(",J35)-1),J32="","")</f>
         <v/>
       </c>
-      <c r="J46" s="28"/>
-      <c r="K46" s="29"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="31"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
@@ -4545,9 +4546,9 @@
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="35"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1" t="str" cm="1">
@@ -5022,7 +5023,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
-      <c r="L59" s="37" t="str" cm="1">
+      <c r="L59" s="28" t="str" cm="1">
         <f t="array" aca="1" ref="L59" ca="1">IF($H$1,INDIRECT("Input!J"&amp;Seeds!F115),"")</f>
         <v/>
       </c>
@@ -33256,7 +33257,7 @@
     <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.08984375" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.08984375" style="27" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.54296875" bestFit="1" customWidth="1"/>
@@ -33295,7 +33296,7 @@
       <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="27" t="s">
         <v>77</v>
       </c>
       <c r="K1" t="s">
@@ -33342,7 +33343,7 @@
       <c r="I2" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="27" t="s">
         <v>88</v>
       </c>
       <c r="K2" t="s">
@@ -33389,7 +33390,7 @@
       <c r="I3" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="27" t="s">
         <v>96</v>
       </c>
       <c r="K3" t="s">
@@ -33436,7 +33437,7 @@
       <c r="I4" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="27" t="s">
         <v>103</v>
       </c>
       <c r="K4" t="s">
@@ -33480,7 +33481,7 @@
       <c r="I5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="27" t="s">
         <v>94</v>
       </c>
       <c r="K5" t="s">
@@ -33518,7 +33519,7 @@
       <c r="I6" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="27" t="s">
         <v>97</v>
       </c>
       <c r="K6" t="s">
@@ -33556,7 +33557,7 @@
       <c r="I7" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="36" t="s">
+      <c r="J7" s="27" t="s">
         <v>114</v>
       </c>
     </row>
@@ -33588,7 +33589,7 @@
       <c r="I8" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="J8" s="27" t="s">
         <v>101</v>
       </c>
     </row>
@@ -33620,7 +33621,7 @@
       <c r="I9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="27" t="s">
         <v>119</v>
       </c>
     </row>
@@ -33652,7 +33653,7 @@
       <c r="I10" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="27" t="s">
         <v>97</v>
       </c>
     </row>
@@ -34303,6 +34304,18 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BDCEF5-57BD-4FF5-9481-792F646FC084}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>